<commit_message>
slides updated + graphs saved from running code
</commit_message>
<xml_diff>
--- a/Datasets/UCD_EngArch_Path_Electronic_ME_Modules.xlsx
+++ b/Datasets/UCD_EngArch_Path_Electronic_ME_Modules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alanh\Documents\GitHub\ChatGPTAssessment\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4546C5A-7386-4475-8A03-5505677C7E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3AE8717-CAE0-4F4E-95B9-9AD6176F4AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C7146B4A-4439-46E0-B60E-DB05B9DBCCC1}"/>
   </bookViews>
@@ -611,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{470AD8BE-D0F1-4863-8083-BF0D6224CD04}">
   <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
UPDATE ELECTRONIC ME MASTERS PATH - REMOVE DUPLICATE MODULES
</commit_message>
<xml_diff>
--- a/Datasets/UCD_EngArch_Path_Electronic_ME_Modules.xlsx
+++ b/Datasets/UCD_EngArch_Path_Electronic_ME_Modules.xlsx
@@ -8,14 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alanh\Documents\GitHub\ChatGPTAssessment\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3AE8717-CAE0-4F4E-95B9-9AD6176F4AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F940C9BC-93BC-4CA3-992B-9377772687A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C7146B4A-4439-46E0-B60E-DB05B9DBCCC1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{C7146B4A-4439-46E0-B60E-DB05B9DBCCC1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$H$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="7" r:id="rId3"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="78">
   <si>
     <t>EEEN20020</t>
   </si>
@@ -245,13 +252,31 @@
     <t>MEEN40430</t>
   </si>
   <si>
-    <t>EEEN40070</t>
-  </si>
-  <si>
-    <t>EEEN40280</t>
-  </si>
-  <si>
-    <t>EEEN40600</t>
+    <t>Sum of Credits</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>(All)</t>
+  </si>
+  <si>
+    <t>EEEN40010</t>
+  </si>
+  <si>
+    <t>EEEN40310</t>
+  </si>
+  <si>
+    <t>EEEN40720</t>
+  </si>
+  <si>
+    <t>COMP47670</t>
+  </si>
+  <si>
+    <t>EEEN40690</t>
   </si>
 </sst>
 </file>
@@ -293,8 +318,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -310,6 +341,735 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Alan Hickey" refreshedDate="45100.430871643519" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="51" xr:uid="{F0F48D58-DE3B-4B1D-85EE-B9FD36F1E8B3}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:H52" sheet="Sheet1"/>
+  </cacheSource>
+  <cacheFields count="8">
+    <cacheField name="Module" numFmtId="0">
+      <sharedItems count="49">
+        <s v="ACM30030"/>
+        <s v="CHEM10030"/>
+        <s v="CHEN10040"/>
+        <s v="COMP10060"/>
+        <s v="COMP20080"/>
+        <s v="COMP20180"/>
+        <s v="COMP20200"/>
+        <s v="COMP41670"/>
+        <s v="CVEN10040"/>
+        <s v="EEEN10010"/>
+        <s v="EEEN10020"/>
+        <s v="EEEN20010"/>
+        <s v="EEEN20020"/>
+        <s v="EEEN20030"/>
+        <s v="EEEN20040"/>
+        <s v="EEEN20050"/>
+        <s v="EEEN20060"/>
+        <s v="EEEN20070"/>
+        <s v="EEEN20090"/>
+        <s v="EEEN30020"/>
+        <s v="EEEN30030"/>
+        <s v="EEEN30050"/>
+        <s v="EEEN30060"/>
+        <s v="EEEN30110"/>
+        <s v="EEEN30120"/>
+        <s v="EEEN30150"/>
+        <s v="EEEN30160"/>
+        <s v="EEEN30190"/>
+        <s v="EEEN40050"/>
+        <s v="EEEN40060"/>
+        <s v="EEEN40070"/>
+        <s v="EEEN40130"/>
+        <s v="EEEN40150"/>
+        <s v="EEEN40210"/>
+        <s v="EEEN40240"/>
+        <s v="EEEN40280"/>
+        <s v="EEEN40570"/>
+        <s v="EEEN40580"/>
+        <s v="EEEN40600"/>
+        <s v="MATH10250"/>
+        <s v="MATH10260"/>
+        <s v="MATH20290"/>
+        <s v="MEEN10030"/>
+        <s v="MEEN10050"/>
+        <s v="MEEN40430"/>
+        <s v="PHYC10150"/>
+        <s v="PHYC10160"/>
+        <s v="SCI20020"/>
+        <s v="STAT20060"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="College" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="School" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Level" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="4"/>
+    </cacheField>
+    <cacheField name="Stage" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="5" count="5">
+        <n v="3"/>
+        <n v="1"/>
+        <n v="2"/>
+        <n v="4"/>
+        <n v="5"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Major" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Credits" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="5" maxValue="30"/>
+    </cacheField>
+    <cacheField name="Trimester" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="51">
+  <r>
+    <x v="0"/>
+    <s v="Science"/>
+    <s v="MathStat"/>
+    <n v="3"/>
+    <x v="0"/>
+    <s v="NES1"/>
+    <n v="5"/>
+    <s v="Aut"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="Science"/>
+    <s v="Chemistry"/>
+    <n v="1"/>
+    <x v="1"/>
+    <s v="NUS1"/>
+    <n v="5"/>
+    <s v="Aut"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="EngArch"/>
+    <s v="ChemEng"/>
+    <n v="1"/>
+    <x v="1"/>
+    <s v="NUS1"/>
+    <n v="5"/>
+    <s v="Aut"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Science"/>
+    <s v="CompSci"/>
+    <n v="1"/>
+    <x v="1"/>
+    <s v="NUS1"/>
+    <n v="5"/>
+    <s v="Spr"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Science"/>
+    <s v="CompSci"/>
+    <n v="3"/>
+    <x v="0"/>
+    <s v="NES1"/>
+    <n v="5"/>
+    <s v="Aut"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="Science"/>
+    <s v="CompSci"/>
+    <n v="3"/>
+    <x v="0"/>
+    <s v="NES1"/>
+    <n v="5"/>
+    <s v="Spr"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <s v="Science"/>
+    <s v="CompSci"/>
+    <n v="2"/>
+    <x v="2"/>
+    <s v="NES1"/>
+    <n v="5"/>
+    <s v="Spr"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <s v="Science"/>
+    <s v="CompSci"/>
+    <n v="4"/>
+    <x v="3"/>
+    <s v="T163"/>
+    <n v="5"/>
+    <s v="Aut"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <s v="Science"/>
+    <s v="CompSci"/>
+    <n v="4"/>
+    <x v="4"/>
+    <s v="T163"/>
+    <n v="5"/>
+    <s v="Aut"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <s v="EngArch"/>
+    <s v="CivEng"/>
+    <n v="1"/>
+    <x v="1"/>
+    <s v="NUS1"/>
+    <n v="5"/>
+    <s v="Aut"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <s v="EngArch"/>
+    <s v="ElecEng"/>
+    <n v="1"/>
+    <x v="1"/>
+    <s v="NUS1"/>
+    <n v="5"/>
+    <s v="Aut"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <s v="EngArch"/>
+    <s v="ElecEng"/>
+    <n v="1"/>
+    <x v="1"/>
+    <s v="NUS1"/>
+    <n v="5"/>
+    <s v="Spr"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <s v="EngArch"/>
+    <s v="ElecEng"/>
+    <n v="2"/>
+    <x v="2"/>
+    <s v="NES1"/>
+    <n v="5"/>
+    <s v="Aut"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <s v="EngArch"/>
+    <s v="ElecEng"/>
+    <n v="2"/>
+    <x v="2"/>
+    <s v="NES1"/>
+    <n v="5"/>
+    <s v="Aut"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <s v="EngArch"/>
+    <s v="ElecEng"/>
+    <n v="2"/>
+    <x v="2"/>
+    <s v="NES1"/>
+    <n v="5"/>
+    <s v="Spr"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <s v="EngArch"/>
+    <s v="ElecEng"/>
+    <n v="2"/>
+    <x v="2"/>
+    <s v="NES1"/>
+    <n v="5"/>
+    <s v="Spr"/>
+  </r>
+  <r>
+    <x v="15"/>
+    <s v="EngArch"/>
+    <s v="ElecEng"/>
+    <n v="2"/>
+    <x v="2"/>
+    <s v="NES1"/>
+    <n v="5"/>
+    <s v="Aut"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <s v="EngArch"/>
+    <s v="ElecEng"/>
+    <n v="2"/>
+    <x v="2"/>
+    <s v="NES1"/>
+    <n v="5"/>
+    <s v="Spr"/>
+  </r>
+  <r>
+    <x v="17"/>
+    <s v="EngArch"/>
+    <s v="ElecEng"/>
+    <n v="2"/>
+    <x v="2"/>
+    <s v="NES1"/>
+    <n v="5"/>
+    <s v="Aut"/>
+  </r>
+  <r>
+    <x v="18"/>
+    <s v="EngArch"/>
+    <s v="ElecEng"/>
+    <n v="2"/>
+    <x v="2"/>
+    <s v="NES1"/>
+    <n v="5"/>
+    <s v="Spr"/>
+  </r>
+  <r>
+    <x v="19"/>
+    <s v="EngArch"/>
+    <s v="ElecEng"/>
+    <n v="3"/>
+    <x v="0"/>
+    <s v="NES1"/>
+    <n v="5"/>
+    <s v="Aut"/>
+  </r>
+  <r>
+    <x v="20"/>
+    <s v="EngArch"/>
+    <s v="ElecEng"/>
+    <n v="3"/>
+    <x v="0"/>
+    <s v="NES1"/>
+    <n v="5"/>
+    <s v="Spr"/>
+  </r>
+  <r>
+    <x v="21"/>
+    <s v="EngArch"/>
+    <s v="ElecEng"/>
+    <n v="3"/>
+    <x v="0"/>
+    <s v="NES1"/>
+    <n v="5"/>
+    <s v="Spr"/>
+  </r>
+  <r>
+    <x v="22"/>
+    <s v="EngArch"/>
+    <s v="ElecEng"/>
+    <n v="3"/>
+    <x v="0"/>
+    <s v="NES1"/>
+    <n v="5"/>
+    <s v="Spr"/>
+  </r>
+  <r>
+    <x v="23"/>
+    <s v="EngArch"/>
+    <s v="ElecEng"/>
+    <n v="3"/>
+    <x v="0"/>
+    <s v="NES1"/>
+    <n v="5"/>
+    <s v="Aut"/>
+  </r>
+  <r>
+    <x v="24"/>
+    <s v="EngArch"/>
+    <s v="ElecEng"/>
+    <n v="3"/>
+    <x v="0"/>
+    <s v="NES1"/>
+    <n v="5"/>
+    <s v="Spr"/>
+  </r>
+  <r>
+    <x v="25"/>
+    <s v="EngArch"/>
+    <s v="ElecEng"/>
+    <n v="3"/>
+    <x v="0"/>
+    <s v="NES1"/>
+    <n v="5"/>
+    <s v="Spr"/>
+  </r>
+  <r>
+    <x v="26"/>
+    <s v="EngArch"/>
+    <s v="ElecEng"/>
+    <n v="3"/>
+    <x v="0"/>
+    <s v="NES1"/>
+    <n v="5"/>
+    <s v="Aut"/>
+  </r>
+  <r>
+    <x v="27"/>
+    <s v="EngArch"/>
+    <s v="ElecEng"/>
+    <n v="3"/>
+    <x v="0"/>
+    <s v="NES1"/>
+    <n v="5"/>
+    <s v="Aut"/>
+  </r>
+  <r>
+    <x v="28"/>
+    <s v="EngArch"/>
+    <s v="ElecEng"/>
+    <n v="4"/>
+    <x v="3"/>
+    <s v="T163"/>
+    <n v="5"/>
+    <s v="Aut"/>
+  </r>
+  <r>
+    <x v="29"/>
+    <s v="EngArch"/>
+    <s v="ElecEng"/>
+    <n v="4"/>
+    <x v="3"/>
+    <s v="T163"/>
+    <n v="5"/>
+    <s v="Aut"/>
+  </r>
+  <r>
+    <x v="29"/>
+    <s v="EngArch"/>
+    <s v="ElecEng"/>
+    <n v="4"/>
+    <x v="4"/>
+    <s v="T163"/>
+    <n v="5"/>
+    <s v="Aut"/>
+  </r>
+  <r>
+    <x v="30"/>
+    <s v="EngArch"/>
+    <s v="ElecEng"/>
+    <n v="4"/>
+    <x v="4"/>
+    <s v="T163"/>
+    <n v="5"/>
+    <s v="Spr"/>
+  </r>
+  <r>
+    <x v="31"/>
+    <s v="EngArch"/>
+    <s v="ElecEng"/>
+    <n v="4"/>
+    <x v="3"/>
+    <s v="T163"/>
+    <n v="5"/>
+    <s v="Aut"/>
+  </r>
+  <r>
+    <x v="32"/>
+    <s v="EngArch"/>
+    <s v="ElecEng"/>
+    <n v="4"/>
+    <x v="3"/>
+    <s v="T163"/>
+    <n v="5"/>
+    <s v="Aut"/>
+  </r>
+  <r>
+    <x v="33"/>
+    <s v="EngArch"/>
+    <s v="ElecEng"/>
+    <n v="4"/>
+    <x v="3"/>
+    <s v="T163"/>
+    <n v="30"/>
+    <s v="Spr"/>
+  </r>
+  <r>
+    <x v="34"/>
+    <s v="EngArch"/>
+    <s v="ElecEng"/>
+    <n v="4"/>
+    <x v="4"/>
+    <s v="T163"/>
+    <n v="25"/>
+    <s v="Aut"/>
+  </r>
+  <r>
+    <x v="35"/>
+    <s v="EngArch"/>
+    <s v="ElecEng"/>
+    <n v="4"/>
+    <x v="4"/>
+    <s v="T163"/>
+    <n v="5"/>
+    <s v="Spr"/>
+  </r>
+  <r>
+    <x v="36"/>
+    <s v="EngArch"/>
+    <s v="ElecEng"/>
+    <n v="4"/>
+    <x v="3"/>
+    <s v="T163"/>
+    <n v="5"/>
+    <s v="Aut"/>
+  </r>
+  <r>
+    <x v="37"/>
+    <s v="EngArch"/>
+    <s v="ElecEng"/>
+    <n v="4"/>
+    <x v="4"/>
+    <s v="T163"/>
+    <n v="5"/>
+    <s v="Aut"/>
+  </r>
+  <r>
+    <x v="38"/>
+    <s v="EngArch"/>
+    <s v="ElecEng"/>
+    <n v="4"/>
+    <x v="4"/>
+    <s v="T163"/>
+    <n v="5"/>
+    <s v="Spr"/>
+  </r>
+  <r>
+    <x v="39"/>
+    <s v="Science"/>
+    <s v="MathStat"/>
+    <n v="1"/>
+    <x v="1"/>
+    <s v="NUS1"/>
+    <n v="5"/>
+    <s v="Aut"/>
+  </r>
+  <r>
+    <x v="40"/>
+    <s v="Science"/>
+    <s v="MathStat"/>
+    <n v="1"/>
+    <x v="1"/>
+    <s v="NUS1"/>
+    <n v="5"/>
+    <s v="Spr"/>
+  </r>
+  <r>
+    <x v="41"/>
+    <s v="Science"/>
+    <s v="MathStat"/>
+    <n v="2"/>
+    <x v="2"/>
+    <s v="NES1"/>
+    <n v="5"/>
+    <s v="Aut"/>
+  </r>
+  <r>
+    <x v="42"/>
+    <s v="EngArch"/>
+    <s v="MechEng"/>
+    <n v="1"/>
+    <x v="1"/>
+    <s v="NUS1"/>
+    <n v="5"/>
+    <s v="Spr"/>
+  </r>
+  <r>
+    <x v="43"/>
+    <s v="EngArch"/>
+    <s v="MechEng"/>
+    <n v="1"/>
+    <x v="1"/>
+    <s v="NUS1"/>
+    <n v="5"/>
+    <s v="Spr"/>
+  </r>
+  <r>
+    <x v="44"/>
+    <s v="EngArch"/>
+    <s v="MechEng"/>
+    <n v="4"/>
+    <x v="4"/>
+    <s v="T163"/>
+    <n v="5"/>
+    <s v="Spr"/>
+  </r>
+  <r>
+    <x v="45"/>
+    <s v="Science"/>
+    <s v="Physics"/>
+    <n v="1"/>
+    <x v="1"/>
+    <s v="NUS1"/>
+    <n v="5"/>
+    <s v="Aut"/>
+  </r>
+  <r>
+    <x v="46"/>
+    <s v="Science"/>
+    <s v="Physics"/>
+    <n v="1"/>
+    <x v="1"/>
+    <s v="NUS1"/>
+    <n v="5"/>
+    <s v="Spr"/>
+  </r>
+  <r>
+    <x v="47"/>
+    <s v="Science"/>
+    <s v="CompSci"/>
+    <n v="2"/>
+    <x v="2"/>
+    <s v="NES1"/>
+    <n v="5"/>
+    <s v="Aut"/>
+  </r>
+  <r>
+    <x v="48"/>
+    <s v="Science"/>
+    <s v="MathStat"/>
+    <n v="2"/>
+    <x v="2"/>
+    <s v="NES1"/>
+    <n v="5"/>
+    <s v="Spr"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EBC335D3-D81C-4F14-B465-9CBC67F70290}" name="PivotTable2" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="8">
+    <pivotField axis="axisPage" showAll="0">
+      <items count="50">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="40"/>
+        <item x="41"/>
+        <item x="42"/>
+        <item x="43"/>
+        <item x="44"/>
+        <item x="45"/>
+        <item x="46"/>
+        <item x="47"/>
+        <item x="48"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="6">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="4"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="0" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Credits" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -608,11 +1368,94 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5C3541D-7A70-4A80-AE25-03A53FA9D139}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="A4:B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="1">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{470AD8BE-D0F1-4863-8083-BF0D6224CD04}">
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="K55" sqref="A27:K55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,13 +1546,13 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -724,18 +1567,18 @@
         <v>5</v>
       </c>
       <c r="H4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -755,13 +1598,13 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -781,13 +1624,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -802,12 +1645,12 @@
         <v>5</v>
       </c>
       <c r="H7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
         <v>33</v>
@@ -828,18 +1671,18 @@
         <v>5</v>
       </c>
       <c r="H8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -859,7 +1702,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
         <v>34</v>
@@ -885,13 +1728,13 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -911,13 +1754,13 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
         <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -932,18 +1775,18 @@
         <v>5</v>
       </c>
       <c r="H12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -963,13 +1806,13 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -984,12 +1827,12 @@
         <v>5</v>
       </c>
       <c r="H14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
         <v>34</v>
@@ -1015,7 +1858,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B16" t="s">
         <v>34</v>
@@ -1039,9 +1882,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B17" t="s">
         <v>34</v>
@@ -1062,18 +1905,18 @@
         <v>5</v>
       </c>
       <c r="H17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D18">
         <v>2</v>
@@ -1088,12 +1931,12 @@
         <v>5</v>
       </c>
       <c r="H18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B19" t="s">
         <v>34</v>
@@ -1114,12 +1957,12 @@
         <v>5</v>
       </c>
       <c r="H19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B20" t="s">
         <v>34</v>
@@ -1143,9 +1986,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B21" t="s">
         <v>34</v>
@@ -1166,10 +2009,10 @@
         <v>5</v>
       </c>
       <c r="H21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>1</v>
       </c>
@@ -1195,9 +2038,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B23" t="s">
         <v>33</v>
@@ -1218,10 +2061,10 @@
         <v>5</v>
       </c>
       <c r="H23" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>47</v>
       </c>
@@ -1247,15 +2090,15 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B25" t="s">
         <v>33</v>
       </c>
       <c r="C25" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D25">
         <v>2</v>
@@ -1273,7 +2116,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>49</v>
       </c>
@@ -1299,683 +2142,805 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="4">
         <v>3</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="4">
         <v>3</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G27">
-        <v>5</v>
-      </c>
-      <c r="H27" t="s">
+      <c r="G27" s="4">
+        <v>5</v>
+      </c>
+      <c r="H27" s="4" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="4">
+        <v>3</v>
+      </c>
+      <c r="E28" s="4">
+        <v>3</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G28" s="4">
+        <v>5</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B28" t="s">
-        <v>34</v>
-      </c>
-      <c r="C28" t="s">
-        <v>30</v>
-      </c>
-      <c r="D28">
+      <c r="B29" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="4">
         <v>3</v>
       </c>
-      <c r="E28">
+      <c r="E29" s="4">
         <v>3</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F29" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G28">
-        <v>5</v>
-      </c>
-      <c r="H28" t="s">
+      <c r="G29" s="4">
+        <v>5</v>
+      </c>
+      <c r="H29" s="4" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" s="4">
+        <v>3</v>
+      </c>
+      <c r="E30" s="4">
+        <v>3</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G30" s="4">
+        <v>5</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="4">
+        <v>3</v>
+      </c>
+      <c r="E31" s="4">
+        <v>3</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G31" s="4">
+        <v>5</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" s="4">
+        <v>3</v>
+      </c>
+      <c r="E32" s="4">
+        <v>3</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G32" s="4">
+        <v>5</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B29" t="s">
-        <v>34</v>
-      </c>
-      <c r="C29" t="s">
-        <v>30</v>
-      </c>
-      <c r="D29">
+      <c r="B33" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D33" s="4">
         <v>3</v>
       </c>
-      <c r="E29">
+      <c r="E33" s="4">
         <v>3</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F33" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G29">
-        <v>5</v>
-      </c>
-      <c r="H29" t="s">
+      <c r="G33" s="4">
+        <v>5</v>
+      </c>
+      <c r="H33" s="4" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>51</v>
-      </c>
-      <c r="B30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C30" t="s">
-        <v>30</v>
-      </c>
-      <c r="D30">
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D34" s="4">
         <v>3</v>
       </c>
-      <c r="E30">
+      <c r="E34" s="4">
         <v>3</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F34" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G30">
-        <v>5</v>
-      </c>
-      <c r="H30" t="s">
+      <c r="G34" s="4">
+        <v>5</v>
+      </c>
+      <c r="H34" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>53</v>
-      </c>
-      <c r="B31" t="s">
-        <v>34</v>
-      </c>
-      <c r="C31" t="s">
-        <v>30</v>
-      </c>
-      <c r="D31">
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D35" s="4">
         <v>3</v>
       </c>
-      <c r="E31">
+      <c r="E35" s="4">
         <v>3</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F35" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G31">
-        <v>5</v>
-      </c>
-      <c r="H31" t="s">
+      <c r="G35" s="4">
+        <v>5</v>
+      </c>
+      <c r="H35" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>52</v>
-      </c>
-      <c r="B32" t="s">
-        <v>34</v>
-      </c>
-      <c r="C32" t="s">
-        <v>30</v>
-      </c>
-      <c r="D32">
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D36" s="4">
         <v>3</v>
       </c>
-      <c r="E32">
+      <c r="E36" s="4">
         <v>3</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F36" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G32">
-        <v>5</v>
-      </c>
-      <c r="H32" t="s">
+      <c r="G36" s="4">
+        <v>5</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37" s="4">
+        <v>3</v>
+      </c>
+      <c r="E37" s="4">
+        <v>3</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G37" s="4">
+        <v>5</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D38" s="4">
+        <v>4</v>
+      </c>
+      <c r="E38" s="4">
+        <v>4</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G38" s="4">
+        <v>5</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D39" s="4">
+        <v>4</v>
+      </c>
+      <c r="E39" s="4">
+        <v>4</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G39" s="4">
+        <v>5</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D40" s="4">
+        <v>4</v>
+      </c>
+      <c r="E40" s="4">
+        <v>4</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G40" s="4">
+        <v>5</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="4"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D41" s="4">
+        <v>4</v>
+      </c>
+      <c r="E41" s="4">
+        <v>4</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G41" s="4">
+        <v>5</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D42" s="4">
+        <v>4</v>
+      </c>
+      <c r="E42" s="4">
+        <v>4</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G42" s="4">
+        <v>5</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="4"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D43" s="4">
+        <v>4</v>
+      </c>
+      <c r="E43" s="4">
+        <v>4</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G43" s="4">
+        <v>5</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="4"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D44" s="4">
+        <v>4</v>
+      </c>
+      <c r="E44" s="4">
+        <v>4</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G44" s="4">
+        <v>30</v>
+      </c>
+      <c r="H44" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>2</v>
-      </c>
-      <c r="B33" t="s">
-        <v>34</v>
-      </c>
-      <c r="C33" t="s">
-        <v>30</v>
-      </c>
-      <c r="D33">
-        <v>3</v>
-      </c>
-      <c r="E33">
-        <v>3</v>
-      </c>
-      <c r="F33" t="s">
-        <v>46</v>
-      </c>
-      <c r="G33">
-        <v>5</v>
-      </c>
-      <c r="H33" t="s">
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="4"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D45" s="4">
+        <v>4</v>
+      </c>
+      <c r="E45" s="4">
+        <v>5</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G45" s="4">
+        <v>25</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I45" s="4"/>
+      <c r="J45" s="4"/>
+      <c r="K45" s="4"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D46" s="4">
+        <v>4</v>
+      </c>
+      <c r="E46" s="4">
+        <v>5</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G46" s="4">
+        <v>5</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4"/>
+      <c r="K46" s="4"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D47" s="4">
+        <v>4</v>
+      </c>
+      <c r="E47" s="4">
+        <v>5</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G47" s="4">
+        <v>5</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I47" s="4"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="4"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D48" s="4">
+        <v>4</v>
+      </c>
+      <c r="E48" s="4">
+        <v>5</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G48" s="4">
+        <v>5</v>
+      </c>
+      <c r="H48" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>54</v>
-      </c>
-      <c r="B34" t="s">
-        <v>34</v>
-      </c>
-      <c r="C34" t="s">
-        <v>30</v>
-      </c>
-      <c r="D34">
-        <v>3</v>
-      </c>
-      <c r="E34">
-        <v>3</v>
-      </c>
-      <c r="F34" t="s">
-        <v>46</v>
-      </c>
-      <c r="G34">
-        <v>5</v>
-      </c>
-      <c r="H34" t="s">
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="4"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D49" s="4">
+        <v>4</v>
+      </c>
+      <c r="E49" s="4">
+        <v>5</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G49" s="4">
+        <v>5</v>
+      </c>
+      <c r="H49" s="4" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>55</v>
-      </c>
-      <c r="B35" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35" t="s">
-        <v>30</v>
-      </c>
-      <c r="D35">
-        <v>3</v>
-      </c>
-      <c r="E35">
-        <v>3</v>
-      </c>
-      <c r="F35" t="s">
-        <v>46</v>
-      </c>
-      <c r="G35">
-        <v>5</v>
-      </c>
-      <c r="H35" t="s">
+      <c r="I49" s="4"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="4"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D50" s="4">
+        <v>4</v>
+      </c>
+      <c r="E50" s="4">
+        <v>5</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G50" s="4">
+        <v>5</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="4"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D51" s="4">
+        <v>4</v>
+      </c>
+      <c r="E51" s="4">
+        <v>5</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G51" s="4">
+        <v>5</v>
+      </c>
+      <c r="H51" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>56</v>
-      </c>
-      <c r="B36" t="s">
-        <v>34</v>
-      </c>
-      <c r="C36" t="s">
-        <v>30</v>
-      </c>
-      <c r="D36">
-        <v>3</v>
-      </c>
-      <c r="E36">
-        <v>3</v>
-      </c>
-      <c r="F36" t="s">
-        <v>46</v>
-      </c>
-      <c r="G36">
-        <v>5</v>
-      </c>
-      <c r="H36" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>57</v>
-      </c>
-      <c r="B37" t="s">
-        <v>33</v>
-      </c>
-      <c r="C37" t="s">
-        <v>42</v>
-      </c>
-      <c r="D37">
-        <v>3</v>
-      </c>
-      <c r="E37">
-        <v>3</v>
-      </c>
-      <c r="F37" t="s">
-        <v>46</v>
-      </c>
-      <c r="G37">
-        <v>5</v>
-      </c>
-      <c r="H37" t="s">
+      <c r="I51" s="4"/>
+      <c r="J51" s="4"/>
+      <c r="K51" s="4"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D52" s="4">
+        <v>4</v>
+      </c>
+      <c r="E52" s="4">
+        <v>5</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G52" s="4">
+        <v>5</v>
+      </c>
+      <c r="H52" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>58</v>
-      </c>
-      <c r="B38" t="s">
-        <v>33</v>
-      </c>
-      <c r="C38" t="s">
-        <v>42</v>
-      </c>
-      <c r="D38">
-        <v>4</v>
-      </c>
-      <c r="E38">
-        <v>4</v>
-      </c>
-      <c r="F38" t="s">
-        <v>59</v>
-      </c>
-      <c r="G38">
-        <v>5</v>
-      </c>
-      <c r="H38" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>60</v>
-      </c>
-      <c r="B39" t="s">
-        <v>34</v>
-      </c>
-      <c r="C39" t="s">
-        <v>30</v>
-      </c>
-      <c r="D39">
-        <v>4</v>
-      </c>
-      <c r="E39">
-        <v>4</v>
-      </c>
-      <c r="F39" t="s">
-        <v>59</v>
-      </c>
-      <c r="G39">
-        <v>5</v>
-      </c>
-      <c r="H39" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>61</v>
-      </c>
-      <c r="B40" t="s">
-        <v>34</v>
-      </c>
-      <c r="C40" t="s">
-        <v>30</v>
-      </c>
-      <c r="D40">
-        <v>4</v>
-      </c>
-      <c r="E40">
-        <v>4</v>
-      </c>
-      <c r="F40" t="s">
-        <v>59</v>
-      </c>
-      <c r="G40">
-        <v>5</v>
-      </c>
-      <c r="H40" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>62</v>
-      </c>
-      <c r="B41" t="s">
-        <v>34</v>
-      </c>
-      <c r="C41" t="s">
-        <v>30</v>
-      </c>
-      <c r="D41">
-        <v>4</v>
-      </c>
-      <c r="E41">
-        <v>4</v>
-      </c>
-      <c r="F41" t="s">
-        <v>59</v>
-      </c>
-      <c r="G41">
-        <v>5</v>
-      </c>
-      <c r="H41" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>63</v>
-      </c>
-      <c r="B42" t="s">
-        <v>34</v>
-      </c>
-      <c r="C42" t="s">
-        <v>30</v>
-      </c>
-      <c r="D42">
-        <v>4</v>
-      </c>
-      <c r="E42">
-        <v>4</v>
-      </c>
-      <c r="F42" t="s">
-        <v>59</v>
-      </c>
-      <c r="G42">
-        <v>5</v>
-      </c>
-      <c r="H42" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>64</v>
-      </c>
-      <c r="B43" t="s">
-        <v>34</v>
-      </c>
-      <c r="C43" t="s">
-        <v>30</v>
-      </c>
-      <c r="D43">
-        <v>4</v>
-      </c>
-      <c r="E43">
-        <v>4</v>
-      </c>
-      <c r="F43" t="s">
-        <v>59</v>
-      </c>
-      <c r="G43">
-        <v>5</v>
-      </c>
-      <c r="H43" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>65</v>
-      </c>
-      <c r="B44" t="s">
-        <v>34</v>
-      </c>
-      <c r="C44" t="s">
-        <v>30</v>
-      </c>
-      <c r="D44">
-        <v>4</v>
-      </c>
-      <c r="E44">
-        <v>4</v>
-      </c>
-      <c r="F44" t="s">
-        <v>59</v>
-      </c>
-      <c r="G44">
-        <v>30</v>
-      </c>
-      <c r="H44" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>66</v>
-      </c>
-      <c r="B45" t="s">
-        <v>34</v>
-      </c>
-      <c r="C45" t="s">
-        <v>30</v>
-      </c>
-      <c r="D45">
-        <v>4</v>
-      </c>
-      <c r="E45">
-        <v>5</v>
-      </c>
-      <c r="F45" t="s">
-        <v>59</v>
-      </c>
-      <c r="G45">
-        <v>25</v>
-      </c>
-      <c r="H45" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>58</v>
-      </c>
-      <c r="B46" t="s">
-        <v>33</v>
-      </c>
-      <c r="C46" t="s">
-        <v>42</v>
-      </c>
-      <c r="D46">
-        <v>4</v>
-      </c>
-      <c r="E46">
-        <v>5</v>
-      </c>
-      <c r="F46" t="s">
-        <v>59</v>
-      </c>
-      <c r="G46">
-        <v>5</v>
-      </c>
-      <c r="H46" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>61</v>
-      </c>
-      <c r="B47" t="s">
-        <v>34</v>
-      </c>
-      <c r="C47" t="s">
-        <v>30</v>
-      </c>
-      <c r="D47">
-        <v>4</v>
-      </c>
-      <c r="E47">
-        <v>5</v>
-      </c>
-      <c r="F47" t="s">
-        <v>59</v>
-      </c>
-      <c r="G47">
-        <v>5</v>
-      </c>
-      <c r="H47" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>67</v>
-      </c>
-      <c r="B48" t="s">
-        <v>34</v>
-      </c>
-      <c r="C48" t="s">
-        <v>30</v>
-      </c>
-      <c r="D48">
-        <v>4</v>
-      </c>
-      <c r="E48">
-        <v>5</v>
-      </c>
-      <c r="F48" t="s">
-        <v>59</v>
-      </c>
-      <c r="G48">
-        <v>5</v>
-      </c>
-      <c r="H48" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>68</v>
-      </c>
-      <c r="B49" t="s">
-        <v>34</v>
-      </c>
-      <c r="C49" t="s">
-        <v>32</v>
-      </c>
-      <c r="D49">
-        <v>4</v>
-      </c>
-      <c r="E49">
-        <v>5</v>
-      </c>
-      <c r="F49" t="s">
-        <v>59</v>
-      </c>
-      <c r="G49">
-        <v>5</v>
-      </c>
-      <c r="H49" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>70</v>
-      </c>
-      <c r="B50" t="s">
-        <v>34</v>
-      </c>
-      <c r="C50" t="s">
-        <v>30</v>
-      </c>
-      <c r="D50">
-        <v>4</v>
-      </c>
-      <c r="E50">
-        <v>5</v>
-      </c>
-      <c r="F50" t="s">
-        <v>59</v>
-      </c>
-      <c r="G50">
-        <v>5</v>
-      </c>
-      <c r="H50" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>71</v>
-      </c>
-      <c r="B51" t="s">
-        <v>34</v>
-      </c>
-      <c r="C51" t="s">
-        <v>30</v>
-      </c>
-      <c r="D51">
-        <v>4</v>
-      </c>
-      <c r="E51">
-        <v>5</v>
-      </c>
-      <c r="F51" t="s">
-        <v>59</v>
-      </c>
-      <c r="G51">
-        <v>5</v>
-      </c>
-      <c r="H51" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>69</v>
-      </c>
-      <c r="B52" t="s">
-        <v>34</v>
-      </c>
-      <c r="C52" t="s">
-        <v>30</v>
-      </c>
-      <c r="D52">
-        <v>4</v>
-      </c>
-      <c r="E52">
-        <v>5</v>
-      </c>
-      <c r="F52" t="s">
-        <v>59</v>
-      </c>
-      <c r="G52">
-        <v>5</v>
-      </c>
-      <c r="H52" t="s">
-        <v>40</v>
-      </c>
+      <c r="I52" s="4"/>
+      <c r="J52" s="4"/>
+      <c r="K52" s="4"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4"/>
+      <c r="K53" s="4"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="4"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="4"/>
+      <c r="J54" s="4"/>
+      <c r="K54" s="4"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="4"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="4"/>
+      <c r="J55" s="4"/>
+      <c r="K55" s="4"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H49" xr:uid="{470AD8BE-D0F1-4863-8083-BF0D6224CD04}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H49">
+      <sortCondition ref="E1"/>
+    </sortState>
+  </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>